<commit_message>
Updated dates in Eli Weinberg Collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/ELI WEINBERG COLLECTION.xlsx
+++ b/Photographic Archive/ELI WEINBERG COLLECTION.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$70</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="169">
   <si>
     <t>identifier</t>
   </si>
@@ -203,9 +206,6 @@
   </si>
   <si>
     <t>HOUSING-CAPE FISHERMAN CA 1936</t>
-  </si>
-  <si>
-    <t>date in title</t>
   </si>
   <si>
     <t>54A-PH</t>
@@ -810,7 +810,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1399,23 +1399,23 @@
       <c r="C20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="5">
+        <v>1936</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
         <v>63</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>64</v>
       </c>
       <c r="N20" t="s">
         <v>24</v>
@@ -1423,13 +1423,13 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>63</v>
+      <c r="D21" s="5">
+        <v>1936</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>11</v>
@@ -1444,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N21" t="s">
         <v>24</v>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>63</v>
+      <c r="D22" s="5">
+        <v>1936</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>11</v>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N22" t="s">
         <v>24</v>
@@ -1481,28 +1481,28 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
         <v>70</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
-        <v>71</v>
       </c>
       <c r="N23" t="s">
         <v>24</v>
@@ -1510,28 +1510,28 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>73</v>
       </c>
       <c r="N24" t="s">
         <v>24</v>
@@ -1539,28 +1539,28 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>75</v>
       </c>
       <c r="N25" t="s">
         <v>24</v>
@@ -1568,28 +1568,28 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
         <v>76</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>77</v>
       </c>
       <c r="N26" t="s">
         <v>24</v>
@@ -1597,28 +1597,28 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>79</v>
       </c>
       <c r="N27" t="s">
         <v>24</v>
@@ -1626,28 +1626,28 @@
     </row>
     <row r="28" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
-        <v>81</v>
       </c>
       <c r="N28" t="s">
         <v>24</v>
@@ -1655,28 +1655,28 @@
     </row>
     <row r="29" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
         <v>83</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
-        <v>84</v>
       </c>
       <c r="N29" t="s">
         <v>24</v>
@@ -1684,28 +1684,28 @@
     </row>
     <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30" t="s">
-        <v>86</v>
       </c>
       <c r="N30" t="s">
         <v>24</v>
@@ -1713,28 +1713,28 @@
     </row>
     <row r="31" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
-        <v>88</v>
       </c>
       <c r="N31" t="s">
         <v>24</v>
@@ -1742,28 +1742,28 @@
     </row>
     <row r="32" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32" t="s">
-        <v>90</v>
       </c>
       <c r="N32" t="s">
         <v>24</v>
@@ -1771,28 +1771,28 @@
     </row>
     <row r="33" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
         <v>91</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
-        <v>92</v>
       </c>
       <c r="N33" t="s">
         <v>24</v>
@@ -1800,28 +1800,28 @@
     </row>
     <row r="34" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
         <v>94</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" t="s">
-        <v>95</v>
       </c>
       <c r="N34" t="s">
         <v>24</v>
@@ -1829,28 +1829,28 @@
     </row>
     <row r="35" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
         <v>96</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35" t="s">
-        <v>97</v>
       </c>
       <c r="N35" t="s">
         <v>24</v>
@@ -1858,28 +1858,28 @@
     </row>
     <row r="36" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
         <v>98</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>99</v>
       </c>
       <c r="N36" t="s">
         <v>24</v>
@@ -1887,28 +1887,28 @@
     </row>
     <row r="37" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
-        <v>101</v>
       </c>
       <c r="N37" t="s">
         <v>24</v>
@@ -1916,28 +1916,28 @@
     </row>
     <row r="38" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38" t="s">
-        <v>103</v>
       </c>
       <c r="N38" t="s">
         <v>24</v>
@@ -1945,28 +1945,28 @@
     </row>
     <row r="39" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39" t="s">
-        <v>105</v>
       </c>
       <c r="N39" t="s">
         <v>24</v>
@@ -1974,28 +1974,28 @@
     </row>
     <row r="40" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
         <v>106</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
-        <v>107</v>
       </c>
       <c r="N40" t="s">
         <v>24</v>
@@ -2003,28 +2003,28 @@
     </row>
     <row r="41" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
         <v>108</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="L41" t="s">
-        <v>109</v>
       </c>
       <c r="N41" t="s">
         <v>24</v>
@@ -2032,28 +2032,28 @@
     </row>
     <row r="42" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
         <v>110</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
-      <c r="L42" t="s">
-        <v>111</v>
       </c>
       <c r="N42" t="s">
         <v>24</v>
@@ -2061,28 +2061,28 @@
     </row>
     <row r="43" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
         <v>112</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K43">
-        <v>1</v>
-      </c>
-      <c r="L43" t="s">
-        <v>113</v>
       </c>
       <c r="N43" t="s">
         <v>24</v>
@@ -2090,28 +2090,28 @@
     </row>
     <row r="44" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
         <v>114</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K44">
-        <v>1</v>
-      </c>
-      <c r="L44" t="s">
-        <v>115</v>
       </c>
       <c r="N44" t="s">
         <v>24</v>
@@ -2119,28 +2119,28 @@
     </row>
     <row r="45" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
         <v>116</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K45">
-        <v>1</v>
-      </c>
-      <c r="L45" t="s">
-        <v>117</v>
       </c>
       <c r="N45" t="s">
         <v>24</v>
@@ -2148,28 +2148,28 @@
     </row>
     <row r="46" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
         <v>118</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K46">
-        <v>1</v>
-      </c>
-      <c r="L46" t="s">
-        <v>119</v>
       </c>
       <c r="N46" t="s">
         <v>24</v>
@@ -2177,28 +2177,28 @@
     </row>
     <row r="47" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
         <v>120</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K47">
-        <v>1</v>
-      </c>
-      <c r="L47" t="s">
-        <v>121</v>
       </c>
       <c r="N47" t="s">
         <v>24</v>
@@ -2206,28 +2206,28 @@
     </row>
     <row r="48" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48" t="s">
         <v>122</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="L48" t="s">
-        <v>123</v>
       </c>
       <c r="N48" t="s">
         <v>24</v>
@@ -2235,28 +2235,28 @@
     </row>
     <row r="49" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
         <v>124</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49" t="s">
-        <v>125</v>
       </c>
       <c r="N49" t="s">
         <v>24</v>
@@ -2264,28 +2264,28 @@
     </row>
     <row r="50" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50" t="s">
         <v>126</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
-      <c r="L50" t="s">
-        <v>127</v>
       </c>
       <c r="N50" t="s">
         <v>24</v>
@@ -2293,28 +2293,28 @@
     </row>
     <row r="51" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51" t="s">
         <v>128</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
-      <c r="L51" t="s">
-        <v>129</v>
       </c>
       <c r="N51" t="s">
         <v>24</v>
@@ -2322,31 +2322,31 @@
     </row>
     <row r="52" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K52">
-        <v>1</v>
-      </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>131</v>
-      </c>
-      <c r="M52" t="s">
-        <v>132</v>
       </c>
       <c r="N52" t="s">
         <v>24</v>
@@ -2354,28 +2354,28 @@
     </row>
     <row r="53" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53" t="s">
         <v>133</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
-      </c>
-      <c r="L53" t="s">
-        <v>134</v>
       </c>
       <c r="N53" t="s">
         <v>24</v>
@@ -2383,28 +2383,28 @@
     </row>
     <row r="54" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
         <v>135</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54" t="s">
-        <v>136</v>
       </c>
       <c r="N54" t="s">
         <v>24</v>
@@ -2412,28 +2412,28 @@
     </row>
     <row r="55" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
         <v>137</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55" t="s">
-        <v>138</v>
       </c>
       <c r="N55" t="s">
         <v>24</v>
@@ -2441,28 +2441,28 @@
     </row>
     <row r="56" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56" t="s">
         <v>139</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K56">
-        <v>1</v>
-      </c>
-      <c r="L56" t="s">
-        <v>140</v>
       </c>
       <c r="N56" t="s">
         <v>24</v>
@@ -2470,28 +2470,28 @@
     </row>
     <row r="57" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57" t="s">
         <v>141</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K57">
-        <v>1</v>
-      </c>
-      <c r="L57" t="s">
-        <v>142</v>
       </c>
       <c r="N57" t="s">
         <v>24</v>
@@ -2499,28 +2499,28 @@
     </row>
     <row r="58" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
         <v>143</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K58">
-        <v>1</v>
-      </c>
-      <c r="L58" t="s">
-        <v>144</v>
       </c>
       <c r="N58" t="s">
         <v>24</v>
@@ -2528,28 +2528,28 @@
     </row>
     <row r="59" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59" t="s">
         <v>145</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59" t="s">
-        <v>146</v>
       </c>
       <c r="N59" t="s">
         <v>24</v>
@@ -2557,28 +2557,28 @@
     </row>
     <row r="60" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60" t="s">
         <v>147</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
-      <c r="L60" t="s">
-        <v>148</v>
       </c>
       <c r="N60" t="s">
         <v>24</v>
@@ -2586,28 +2586,28 @@
     </row>
     <row r="61" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61" t="s">
         <v>149</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
-      <c r="L61" t="s">
-        <v>150</v>
       </c>
       <c r="N61" t="s">
         <v>24</v>
@@ -2615,28 +2615,28 @@
     </row>
     <row r="62" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
         <v>151</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K62">
-        <v>1</v>
-      </c>
-      <c r="L62" t="s">
-        <v>152</v>
       </c>
       <c r="N62" t="s">
         <v>24</v>
@@ -2644,28 +2644,28 @@
     </row>
     <row r="63" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63" t="s">
         <v>153</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K63">
-        <v>1</v>
-      </c>
-      <c r="L63" t="s">
-        <v>154</v>
       </c>
       <c r="N63" t="s">
         <v>24</v>
@@ -2673,28 +2673,28 @@
     </row>
     <row r="64" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64" t="s">
         <v>155</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K64">
-        <v>1</v>
-      </c>
-      <c r="L64" t="s">
-        <v>156</v>
       </c>
       <c r="N64" t="s">
         <v>24</v>
@@ -2702,28 +2702,28 @@
     </row>
     <row r="65" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65" t="s">
         <v>157</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K65">
-        <v>1</v>
-      </c>
-      <c r="L65" t="s">
-        <v>158</v>
       </c>
       <c r="N65" t="s">
         <v>24</v>
@@ -2731,28 +2731,28 @@
     </row>
     <row r="66" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
         <v>159</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K66">
-        <v>1</v>
-      </c>
-      <c r="L66" t="s">
-        <v>160</v>
       </c>
       <c r="N66" t="s">
         <v>24</v>
@@ -2760,28 +2760,28 @@
     </row>
     <row r="67" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
         <v>161</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K67">
-        <v>1</v>
-      </c>
-      <c r="L67" t="s">
-        <v>162</v>
       </c>
       <c r="N67" t="s">
         <v>24</v>
@@ -2789,28 +2789,28 @@
     </row>
     <row r="68" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
         <v>163</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
-      <c r="L68" t="s">
-        <v>164</v>
       </c>
       <c r="N68" t="s">
         <v>24</v>
@@ -2818,31 +2818,31 @@
     </row>
     <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D69" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69" t="s">
+        <v>22</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
         <v>165</v>
       </c>
-      <c r="C69" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" t="s">
-        <v>20</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>21</v>
-      </c>
-      <c r="G69" t="s">
-        <v>22</v>
-      </c>
-      <c r="K69">
-        <v>1</v>
-      </c>
-      <c r="L69" t="s">
+      <c r="M69" t="s">
         <v>166</v>
-      </c>
-      <c r="M69" t="s">
-        <v>167</v>
       </c>
       <c r="N69" t="s">
         <v>24</v>
@@ -2850,34 +2850,35 @@
     </row>
     <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s">
+        <v>21</v>
+      </c>
+      <c r="G70" t="s">
+        <v>22</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
         <v>168</v>
       </c>
-      <c r="C70" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" t="s">
-        <v>21</v>
-      </c>
-      <c r="G70" t="s">
-        <v>22</v>
-      </c>
-      <c r="K70">
-        <v>1</v>
-      </c>
-      <c r="L70" t="s">
-        <v>169</v>
-      </c>
       <c r="N70" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z70"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed collection data from Eli Weinberg collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/ELI WEINBERG COLLECTION.xlsx
+++ b/Photographic Archive/ELI WEINBERG COLLECTION.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="167">
   <si>
     <t>identifier</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>37A-PH</t>
-  </si>
-  <si>
-    <t>WEINBERG, Eli</t>
   </si>
   <si>
     <t>EW203-1-3</t>
@@ -806,8 +803,8 @@
   <dimension ref="A1:Z70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -919,13 +916,10 @@
       <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>19</v>
@@ -944,15 +938,12 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>
@@ -971,15 +962,12 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>19</v>
@@ -998,15 +986,12 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>19</v>
@@ -1025,18 +1010,15 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
@@ -1052,45 +1034,39 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>38</v>
-      </c>
-      <c r="N9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
@@ -1106,18 +1082,15 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
@@ -1133,18 +1106,15 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
@@ -1160,18 +1130,15 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
@@ -1187,18 +1154,15 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
@@ -1214,25 +1178,22 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>21</v>
@@ -1241,18 +1202,15 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
@@ -1268,18 +1226,15 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
@@ -1295,18 +1250,15 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="N17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
@@ -1322,18 +1274,15 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6" t="s">
@@ -1349,18 +1298,15 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D20" s="5">
         <v>1936</v>
@@ -1378,18 +1324,15 @@
         <v>1</v>
       </c>
       <c r="L20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="5">
         <v>1936</v>
@@ -1407,18 +1350,15 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="5">
         <v>1936</v>
@@ -1436,18 +1376,15 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="N22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
@@ -1463,18 +1400,15 @@
         <v>1</v>
       </c>
       <c r="L23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="N23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
@@ -1490,18 +1424,15 @@
         <v>1</v>
       </c>
       <c r="L24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
@@ -1517,18 +1448,15 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="N25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="6" t="s">
@@ -1544,18 +1472,15 @@
         <v>1</v>
       </c>
       <c r="L26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="C27" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="s">
@@ -1571,18 +1496,15 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
@@ -1598,18 +1520,15 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="6" t="s">
@@ -1625,18 +1544,15 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="N29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
@@ -1652,18 +1568,15 @@
         <v>1</v>
       </c>
       <c r="L30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="6" t="s">
@@ -1679,18 +1592,15 @@
         <v>1</v>
       </c>
       <c r="L31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="N31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="s">
@@ -1706,18 +1616,15 @@
         <v>1</v>
       </c>
       <c r="L32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="C33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="s">
@@ -1733,18 +1640,15 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="6" t="s">
@@ -1760,18 +1664,15 @@
         <v>1</v>
       </c>
       <c r="L34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
@@ -1787,18 +1688,15 @@
         <v>1</v>
       </c>
       <c r="L35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C36" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
@@ -1814,18 +1712,15 @@
         <v>1</v>
       </c>
       <c r="L36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="N36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C37" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
@@ -1841,18 +1736,15 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="N37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C38" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
@@ -1868,18 +1760,15 @@
         <v>1</v>
       </c>
       <c r="L38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C39" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6" t="s">
@@ -1895,18 +1784,15 @@
         <v>1</v>
       </c>
       <c r="L39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="N39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6" t="s">
@@ -1922,18 +1808,15 @@
         <v>1</v>
       </c>
       <c r="L40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="N40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C41" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6" t="s">
@@ -1949,18 +1832,15 @@
         <v>1</v>
       </c>
       <c r="L41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="C42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="6" t="s">
@@ -1976,18 +1856,15 @@
         <v>1</v>
       </c>
       <c r="L42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="C43" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
@@ -2003,18 +1880,15 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="N43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="6" t="s">
@@ -2030,18 +1904,15 @@
         <v>1</v>
       </c>
       <c r="L44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="N44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="6" t="s">
@@ -2057,18 +1928,15 @@
         <v>1</v>
       </c>
       <c r="L45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="N45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="6" t="s">
@@ -2084,18 +1952,15 @@
         <v>1</v>
       </c>
       <c r="L46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="N46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C47" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="6" t="s">
@@ -2111,18 +1976,15 @@
         <v>1</v>
       </c>
       <c r="L47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="C48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="6" t="s">
@@ -2138,18 +2000,15 @@
         <v>1</v>
       </c>
       <c r="L48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="C49" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="6" t="s">
@@ -2165,18 +2024,15 @@
         <v>1</v>
       </c>
       <c r="L49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="N49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="6" t="s">
@@ -2192,18 +2048,15 @@
         <v>1</v>
       </c>
       <c r="L50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="6" t="s">
@@ -2219,18 +2072,15 @@
         <v>1</v>
       </c>
       <c r="L51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="N51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C52" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="6" t="s">
@@ -2246,21 +2096,18 @@
         <v>1</v>
       </c>
       <c r="L52" t="s">
+        <v>128</v>
+      </c>
+      <c r="M52" t="s">
         <v>129</v>
       </c>
-      <c r="M52" t="s">
+    </row>
+    <row r="53" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="N52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="6" t="s">
@@ -2276,18 +2123,15 @@
         <v>1</v>
       </c>
       <c r="L53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="N53" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="C54" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="6" t="s">
@@ -2303,18 +2147,15 @@
         <v>1</v>
       </c>
       <c r="L54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="N54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="C55" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="s">
@@ -2330,18 +2171,15 @@
         <v>1</v>
       </c>
       <c r="L55" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="N55" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="C56" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="6" t="s">
@@ -2357,18 +2195,15 @@
         <v>1</v>
       </c>
       <c r="L56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="N56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="C57" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="6" t="s">
@@ -2384,18 +2219,15 @@
         <v>1</v>
       </c>
       <c r="L57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="N57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="C58" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="6" t="s">
@@ -2411,18 +2243,15 @@
         <v>1</v>
       </c>
       <c r="L58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="N58" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="C59" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="6" t="s">
@@ -2438,18 +2267,15 @@
         <v>1</v>
       </c>
       <c r="L59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="N59" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="C60" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="6" t="s">
@@ -2465,18 +2291,15 @@
         <v>1</v>
       </c>
       <c r="L60" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="N60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="C61" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="6" t="s">
@@ -2492,18 +2315,15 @@
         <v>1</v>
       </c>
       <c r="L61" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="N61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C62" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="6" t="s">
@@ -2519,18 +2339,15 @@
         <v>1</v>
       </c>
       <c r="L62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N62" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="6" t="s">
@@ -2546,18 +2363,15 @@
         <v>1</v>
       </c>
       <c r="L63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="N63" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="C64" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="6" t="s">
@@ -2573,18 +2387,15 @@
         <v>1</v>
       </c>
       <c r="L64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N64" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="C65" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="6" t="s">
@@ -2600,18 +2411,15 @@
         <v>1</v>
       </c>
       <c r="L65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="N65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="C66" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="6" t="s">
@@ -2627,18 +2435,15 @@
         <v>1</v>
       </c>
       <c r="L66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="N66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="C67" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="6" t="s">
@@ -2654,18 +2459,15 @@
         <v>1</v>
       </c>
       <c r="L67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="N67" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="C68" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="6" t="s">
@@ -2681,65 +2483,56 @@
         <v>1</v>
       </c>
       <c r="L68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>162</v>
       </c>
-      <c r="N68" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" t="s">
+        <v>21</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
         <v>163</v>
       </c>
-      <c r="C69" t="s">
-        <v>92</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>20</v>
-      </c>
-      <c r="G69" t="s">
-        <v>21</v>
-      </c>
-      <c r="K69">
-        <v>1</v>
-      </c>
-      <c r="L69" t="s">
+      <c r="M69" t="s">
         <v>164</v>
       </c>
-      <c r="M69" t="s">
+    </row>
+    <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>165</v>
       </c>
-      <c r="N69" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="C70" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="s">
+        <v>21</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
         <v>166</v>
-      </c>
-      <c r="C70" t="s">
-        <v>92</v>
-      </c>
-      <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" t="s">
-        <v>21</v>
-      </c>
-      <c r="K70">
-        <v>1</v>
-      </c>
-      <c r="L70" t="s">
-        <v>167</v>
-      </c>
-      <c r="N70" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>